<commit_message>
Added Test cases in BWP Bootstrap
</commit_message>
<xml_diff>
--- a/KatalonData/BWPBootstrapData/BWPACHData.xlsx
+++ b/KatalonData/BWPBootstrapData/BWPACHData.xlsx
@@ -8,35 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476046\Documents\VPS-Katalon-feature-VRelay\KatalonData\BWPBootstrapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{7964AC05-494F-4E23-B86D-15D2742C1D3C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{6358A1C5-9A9A-411E-9528-46E9D2F62F3C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="23" firstSheet="19" windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
+    <workbookView activeTab="12" firstSheet="9" windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="PayNowCorpNoCF" r:id="rId1" sheetId="1"/>
     <sheet name="PayNowCorpNoCFOnly" r:id="rId2" sheetId="13"/>
-    <sheet name="PayNowCorpSCF" r:id="rId3" sheetId="7"/>
-    <sheet name="MaxAmountErrorCorp" r:id="rId4" sheetId="19"/>
-    <sheet name="MinAmountErrorCorp" r:id="rId5" sheetId="22"/>
-    <sheet name="PayNowCorpDCF" r:id="rId6" sheetId="8"/>
-    <sheet name="NoModifyAmountCorp" r:id="rId7" sheetId="16"/>
-    <sheet name="PayNowCorpNoCFReqFields" r:id="rId8" sheetId="2"/>
-    <sheet name="PayNowPCSCF" r:id="rId9" sheetId="9"/>
-    <sheet name="PayNowPCDCF" r:id="rId10" sheetId="11"/>
-    <sheet name="PayNowPCNoCF" r:id="rId11" sheetId="3"/>
-    <sheet name="PayNowPCNoCFOnly" r:id="rId12" sheetId="14"/>
-    <sheet name="MinAmountErrorPC" r:id="rId13" sheetId="23"/>
-    <sheet name="MaxAmountErrorPC" r:id="rId14" sheetId="20"/>
-    <sheet name="PayNowPCNoCFReqFields" r:id="rId15" sheetId="4"/>
-    <sheet name="PayNowPSNoCFOnly" r:id="rId16" sheetId="15"/>
-    <sheet name="NoModifyAmountPC" r:id="rId17" sheetId="17"/>
-    <sheet name="PayNowPSNoCF" r:id="rId18" sheetId="5"/>
-    <sheet name="PayNowPSNoCFReqFields" r:id="rId19" sheetId="6"/>
+    <sheet name="ACMismatchCorp" r:id="rId3" sheetId="25"/>
+    <sheet name="PayNowCorpDCF" r:id="rId4" sheetId="8"/>
+    <sheet name="PayNowCorpSCF" r:id="rId5" sheetId="7"/>
+    <sheet name="MaxAmountErrorCorp" r:id="rId6" sheetId="19"/>
+    <sheet name="MinAmountErrorCorp" r:id="rId7" sheetId="22"/>
+    <sheet name="NoModifyAmountCorp" r:id="rId8" sheetId="16"/>
+    <sheet name="PayNowCorpNoCFReqFields" r:id="rId9" sheetId="2"/>
+    <sheet name="PayNowPCNoCF" r:id="rId10" sheetId="3"/>
+    <sheet name="PayNowPCSCF" r:id="rId11" sheetId="9"/>
+    <sheet name="PayNowPCDCF" r:id="rId12" sheetId="11"/>
+    <sheet name="ACMismatchPC" r:id="rId13" sheetId="26"/>
+    <sheet name="PayNowPCNoCFReqFields" r:id="rId14" sheetId="4"/>
+    <sheet name="PayNowPCNoCFOnly" r:id="rId15" sheetId="14"/>
+    <sheet name="NoModifyAmountPC" r:id="rId16" sheetId="17"/>
+    <sheet name="MinAmountErrorPC" r:id="rId17" sheetId="23"/>
+    <sheet name="MaxAmountErrorPC" r:id="rId18" sheetId="20"/>
+    <sheet name="PayNowPSNoCF" r:id="rId19" sheetId="5"/>
     <sheet name="PayNowPSSCF" r:id="rId20" sheetId="10"/>
     <sheet name="PayNowPSDCF" r:id="rId21" sheetId="12"/>
-    <sheet name="NoModifyAmountPS" r:id="rId22" sheetId="18"/>
-    <sheet name="MaxAmountErrorPS" r:id="rId23" sheetId="21"/>
-    <sheet name="MinAmountErrorPS" r:id="rId24" sheetId="24"/>
+    <sheet name="PayNowPSNoCFOnly" r:id="rId22" sheetId="15"/>
+    <sheet name="PayNowPSNoCFReqFields" r:id="rId23" sheetId="6"/>
+    <sheet name="NoModifyAmountPS" r:id="rId24" sheetId="18"/>
+    <sheet name="MaxAmountErrorPS" r:id="rId25" sheetId="21"/>
+    <sheet name="MinAmountErrorPS" r:id="rId26" sheetId="24"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="63">
   <si>
     <t>Result</t>
   </si>
@@ -197,9 +199,6 @@
     <t>Tue Oct 07 21:52:01 IST 2025</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>Wed Oct 08 21:14:53 IST 2025</t>
   </si>
   <si>
@@ -209,19 +208,37 @@
     <t>Wed Oct 08 22:09:25 IST 2025</t>
   </si>
   <si>
-    <t>12</t>
+    <t>Thu Oct 09 19:26:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Oct 09 19:32:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Oct 09 19:35:02 IST 2025</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Thu Oct 09 19:26:42 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Oct 09 19:32:16 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Oct 09 19:35:02 IST 2025</t>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 19:32:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 19:34:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 19:36:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 20:38:00 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -664,103 +681,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35ACE39D-499D-49B4-BFD2-CDDE6D0F8728}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84B2224-A06F-477C-8FF6-AF4C244AA0CE}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -860,7 +780,394 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C366B0B2-5D78-426C-AEBB-C29C53584E7F}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="A1:N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35ACE39D-499D-49B4-BFD2-CDDE6D0F8728}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="A1:N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29FACBAA-68A5-4A1D-8E32-A4AA8B032AE1}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F93338-8AAA-4B19-8B9D-4771302FEFC0}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" customWidth="true" width="17.21875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EC6E653-D4E4-4FCF-8BD0-11D4CBABA3A9}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -960,397 +1267,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CD5E31-F635-4FC0-9668-1419F01D6942}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD2F0AE-7828-442C-A2B3-21D0EBE7331D}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="A1:N2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.44140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F93338-8AAA-4B19-8B9D-4771302FEFC0}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="A1:N2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" customWidth="true" width="17.21875" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D307F9B9-84A6-4F70-AF5F-E09C0B70177D}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF98BAE0-3DBA-4724-A623-84E06EAD3F5D}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -1450,7 +1367,204 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CD5E31-F635-4FC0-9668-1419F01D6942}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD2F0AE-7828-442C-A2B3-21D0EBE7331D}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.44140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E2C147-58C7-49F8-940A-3E37DE049451}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -1533,99 +1647,6 @@
       </c>
       <c r="K2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CED210A-15BA-4154-A75C-369A0BF113DA}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
@@ -1934,6 +1955,196 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D307F9B9-84A6-4F70-AF5F-E09C0B70177D}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CED210A-15BA-4154-A75C-369A0BF113DA}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CCEC20-911A-47BC-B790-0438DD3BE26D}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -2030,8 +2241,299 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE927C8-204D-43C3-9530-F9F77785B40B}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAABB2E9-54E4-4860-85B4-28F35D889E47}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CB3A07-E958-4D14-B792-C4C5D72CD8EA}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893E9D9E-A65A-420C-985F-4AFBCEBD5458}">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2089,17 +2591,17 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>16</v>
@@ -2109,16 +2611,16 @@
         <v>17</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2127,104 +2629,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAABB2E9-54E4-4860-85B4-28F35D889E47}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F88BD42D-CC7A-48FA-8796-B59D2B587379}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -2321,12 +2726,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B65B44A-04F0-4B2C-962C-6C956F0737B9}">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:N2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2383,14 +2788,14 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>15</v>
@@ -2421,7 +2826,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A462096B-4AF9-4B81-B6B6-00EE8E7EF270}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -2480,14 +2885,14 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>15</v>
@@ -2518,104 +2923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893E9D9E-A65A-420C-985F-4AFBCEBD5458}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E9BD2B-9C3A-4D4A-991E-C6044AE36784}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -2715,12 +3023,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A723C119-E528-48BF-99DE-522307C92146}">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2786,7 +3094,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>15</v>
@@ -2803,103 +3111,6 @@
       </c>
       <c r="K2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C366B0B2-5D78-426C-AEBB-C29C53584E7F}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="A1:N2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">

</xml_diff>

<commit_message>
BWP Bootstrap Test cases added
</commit_message>
<xml_diff>
--- a/KatalonData/BWPBootstrapData/BWPACHData.xlsx
+++ b/KatalonData/BWPBootstrapData/BWPACHData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476046\Documents\VPS-Katalon-feature-VRelay\KatalonData\BWPBootstrapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{6358A1C5-9A9A-411E-9528-46E9D2F62F3C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{A7D9CA11-21A9-4FF3-8818-C427BB2408CE}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="12" firstSheet="9" windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
+    <workbookView activeTab="24" firstSheet="21" windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="PayNowCorpNoCF" r:id="rId1" sheetId="1"/>
@@ -26,19 +26,37 @@
     <sheet name="PayNowPCSCF" r:id="rId11" sheetId="9"/>
     <sheet name="PayNowPCDCF" r:id="rId12" sheetId="11"/>
     <sheet name="ACMismatchPC" r:id="rId13" sheetId="26"/>
-    <sheet name="PayNowPCNoCFReqFields" r:id="rId14" sheetId="4"/>
-    <sheet name="PayNowPCNoCFOnly" r:id="rId15" sheetId="14"/>
-    <sheet name="NoModifyAmountPC" r:id="rId16" sheetId="17"/>
-    <sheet name="MinAmountErrorPC" r:id="rId17" sheetId="23"/>
-    <sheet name="MaxAmountErrorPC" r:id="rId18" sheetId="20"/>
-    <sheet name="PayNowPSNoCF" r:id="rId19" sheetId="5"/>
-    <sheet name="PayNowPSSCF" r:id="rId20" sheetId="10"/>
-    <sheet name="PayNowPSDCF" r:id="rId21" sheetId="12"/>
-    <sheet name="PayNowPSNoCFOnly" r:id="rId22" sheetId="15"/>
-    <sheet name="PayNowPSNoCFReqFields" r:id="rId23" sheetId="6"/>
-    <sheet name="NoModifyAmountPS" r:id="rId24" sheetId="18"/>
-    <sheet name="MaxAmountErrorPS" r:id="rId25" sheetId="21"/>
-    <sheet name="MinAmountErrorPS" r:id="rId26" sheetId="24"/>
+    <sheet name="DualCFCeilingCorp" r:id="rId14" sheetId="27"/>
+    <sheet name="DualCFCeilingPC" r:id="rId15" sheetId="28"/>
+    <sheet name="DualCFCeilingPS" r:id="rId16" sheetId="29"/>
+    <sheet name="DualCFFlatCorp" r:id="rId17" sheetId="30"/>
+    <sheet name="DualCFFlatPC" r:id="rId18" sheetId="31"/>
+    <sheet name="DualCFFlatPS" r:id="rId19" sheetId="32"/>
+    <sheet name="DualCFPercentageCorp" r:id="rId20" sheetId="33"/>
+    <sheet name="DualCFPercentagePC" r:id="rId21" sheetId="34"/>
+    <sheet name="DualCFPercentagePS" r:id="rId22" sheetId="35"/>
+    <sheet name="SingleCFCeilingCorp" r:id="rId23" sheetId="36"/>
+    <sheet name="SingleCFCeilingPS" r:id="rId24" sheetId="38"/>
+    <sheet name="SingleCFCeilingPC" r:id="rId25" sheetId="37"/>
+    <sheet name="SingleCFFlatCorp" r:id="rId26" sheetId="39"/>
+    <sheet name="SingleCFFlatPC" r:id="rId27" sheetId="40"/>
+    <sheet name="SingleCFFlatPS" r:id="rId28" sheetId="41"/>
+    <sheet name="SingleCFPercentageCorp" r:id="rId29" sheetId="42"/>
+    <sheet name="SingleCFPercentagePC" r:id="rId30" sheetId="43"/>
+    <sheet name="SingleCFPercentagePS" r:id="rId31" sheetId="44"/>
+    <sheet name="PayNowPCNoCFReqFields" r:id="rId32" sheetId="4"/>
+    <sheet name="PayNowPCNoCFOnly" r:id="rId33" sheetId="14"/>
+    <sheet name="NoModifyAmountPC" r:id="rId34" sheetId="17"/>
+    <sheet name="MinAmountErrorPC" r:id="rId35" sheetId="23"/>
+    <sheet name="MaxAmountErrorPC" r:id="rId36" sheetId="20"/>
+    <sheet name="PayNowPSNoCF" r:id="rId37" sheetId="5"/>
+    <sheet name="PayNowPSSCF" r:id="rId38" sheetId="10"/>
+    <sheet name="PayNowPSDCF" r:id="rId39" sheetId="12"/>
+    <sheet name="PayNowPSNoCFOnly" r:id="rId40" sheetId="15"/>
+    <sheet name="PayNowPSNoCFReqFields" r:id="rId41" sheetId="6"/>
+    <sheet name="NoModifyAmountPS" r:id="rId42" sheetId="18"/>
+    <sheet name="MaxAmountErrorPS" r:id="rId43" sheetId="21"/>
+    <sheet name="MinAmountErrorPS" r:id="rId44" sheetId="24"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -50,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="84">
   <si>
     <t>Result</t>
   </si>
@@ -223,22 +241,85 @@
     <t>7</t>
   </si>
   <si>
+    <t>Mon Oct 13 19:36:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Oct 13 20:38:00 IST 2025</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Tue Nov 04 23:59:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Nov 05 00:07:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Nov 05 00:24:14 IST 2025</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Wed Nov 05 19:36:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Nov 05 19:42:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Nov 05 19:48:45 IST 2025</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Wed Nov 05 20:49:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Nov 05 20:52:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 06 21:50:00 IST 2025</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 20:38:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 20:40:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 20:42:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 20:44:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 20:53:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 20:55:46 IST 2025</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Mon Oct 13 19:32:39 IST 2025</t>
-  </si>
-  <si>
-    <t>Mon Oct 13 19:34:40 IST 2025</t>
-  </si>
-  <si>
-    <t>Mon Oct 13 19:36:00 IST 2025</t>
-  </si>
-  <si>
-    <t>Mon Oct 13 20:38:00 IST 2025</t>
+    <t>Mon Nov 10 21:06:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 21:07:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 21:09:02 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -882,7 +963,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="A1:N2"/>
+      <selection activeCell="F2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,7 +1059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29FACBAA-68A5-4A1D-8E32-A4AA8B032AE1}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -1033,7 +1114,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1072,307 +1153,11 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F93338-8AAA-4B19-8B9D-4771302FEFC0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{924F2B64-1D9A-415C-B98F-EB7A7BAB8DD9}">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" customWidth="true" width="17.21875" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EC6E653-D4E4-4FCF-8BD0-11D4CBABA3A9}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="A1:N2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.44140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF98BAE0-3DBA-4724-A623-84E06EAD3F5D}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.44140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CD5E31-F635-4FC0-9668-1419F01D6942}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1426,17 +1211,17 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>16</v>
@@ -1446,16 +1231,16 @@
         <v>17</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1464,112 +1249,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD2F0AE-7828-442C-A2B3-21D0EBE7331D}">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A084124A-76B7-4B99-A6AD-5B2A169F9B8A}">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.44140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E2C147-58C7-49F8-940A-3E37DE049451}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="A1:XFD1048576"/>
+      <selection activeCell="E2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1623,17 +1308,17 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="3"/>
+        <v>61</v>
+      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>16</v>
@@ -1646,13 +1331,401 @@
         <v>14</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0332CA16-31EB-4917-9936-860E79D3523B}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1E53DD-391D-45C7-A26E-A3CBEF12F623}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65676D18-4455-410B-8CF0-024536C3D41C}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06203600-C68B-4759-93E3-003ACDDD00D9}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1761,11 +1834,11 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC79200-E4B3-4160-86F6-78B06F6EA2C0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{044EB785-1D8B-4520-A589-98FB5248CE3B}">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="A1:N2"/>
+      <selection activeCell="A2" sqref="A1:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1819,17 +1892,17 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>16</v>
@@ -1839,10 +1912,10 @@
         <v>17</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
@@ -1858,7 +1931,492 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{026E9C75-7C58-441D-91D6-25552A135B0A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB2259B-110A-4E54-AAE6-DB14B9EB5171}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="A1:N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE735932-BE48-4F0B-B6E0-1AACE863DBE6}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="A1:N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4FDA41C-A48E-4DF7-9F3C-4EA15B85EA24}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6653DFE2-5232-47EC-B0F1-E3DFB6BF3E7A}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C026E37F-098F-42E5-92AB-1E317624CC4D}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB610E4-D8A9-4F86-99AA-691BCAA68B9C}">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1916,17 +2474,17 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>16</v>
@@ -1936,10 +2494,10 @@
         <v>17</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
@@ -1954,12 +2512,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D307F9B9-84A6-4F70-AF5F-E09C0B70177D}">
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3C025A-C3F4-4ABF-9C60-AA1DCCB0BC50}">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2013,17 +2571,17 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="3"/>
+        <v>76</v>
+      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>16</v>
@@ -2036,13 +2594,13 @@
         <v>14</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2051,8 +2609,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CED210A-15BA-4154-A75C-369A0BF113DA}">
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A067396-2824-448F-9289-4B8D3E2041FE}">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2106,17 +2664,21 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C2" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>16</v>
@@ -2129,13 +2691,13 @@
         <v>14</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2144,12 +2706,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CCEC20-911A-47BC-B790-0438DD3BE26D}">
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AECE1F9-32F0-48E5-B835-168A7EF42FA8}">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2203,17 +2765,17 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>16</v>
@@ -2223,210 +2785,16 @@
         <v>17</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE927C8-204D-43C3-9530-F9F77785B40B}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAABB2E9-54E4-4860-85B4-28F35D889E47}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2494,7 +2862,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2532,8 +2900,889 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893E9D9E-A65A-420C-985F-4AFBCEBD5458}">
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEB8BAF-D441-4510-B01C-E6A2F0E35EEA}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4CCB5A6-D07A-4BC3-BD3B-767113A862D2}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F93338-8AAA-4B19-8B9D-4771302FEFC0}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" customWidth="true" width="17.21875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EC6E653-D4E4-4FCF-8BD0-11D4CBABA3A9}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="A1:N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.44140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF98BAE0-3DBA-4724-A623-84E06EAD3F5D}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.44140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CD5E31-F635-4FC0-9668-1419F01D6942}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD2F0AE-7828-442C-A2B3-21D0EBE7331D}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.44140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E2C147-58C7-49F8-940A-3E37DE049451}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC79200-E4B3-4160-86F6-78B06F6EA2C0}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="A1:N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{026E9C75-7C58-441D-91D6-25552A135B0A}">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2591,7 +3840,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2611,16 +3860,594 @@
         <v>17</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893E9D9E-A65A-420C-985F-4AFBCEBD5458}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D307F9B9-84A6-4F70-AF5F-E09C0B70177D}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CED210A-15BA-4154-A75C-369A0BF113DA}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CCEC20-911A-47BC-B790-0438DD3BE26D}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE927C8-204D-43C3-9530-F9F77785B40B}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAABB2E9-54E4-4860-85B4-28F35D889E47}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes during Regression Testing
</commit_message>
<xml_diff>
--- a/KatalonData/BWPBootstrapData/BWPACHData.xlsx
+++ b/KatalonData/BWPBootstrapData/BWPACHData.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="171">
   <si>
     <t>Result</t>
   </si>
@@ -320,6 +320,267 @@
   </si>
   <si>
     <t>Mon Nov 10 21:09:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 22:50:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 22:51:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 22:53:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 22:54:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 22:54:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 22:55:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 22:56:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 22:56:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:08:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:09:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:11:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:12:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:14:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:15:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:18:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:19:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:20:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:21:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:22:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:23:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:25:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:25:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:27:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:30:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:32:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:36:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:38:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:39:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:41:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:43:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:44:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:46:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:47:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:48:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:51:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:53:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:54:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:54:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:55:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:57:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:58:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 20 23:59:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:00:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:02:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:04:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:05:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:07:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:08:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:11:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:12:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:14:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:15:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:18:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:20:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:30:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:31:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:35:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:37:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:37:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:39:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:40:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:41:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:42:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:43:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:44:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:45:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:46:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:47:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:48:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:50:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:52:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:54:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:57:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 00:58:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 01:00:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 01:01:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 01:01:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 01:04:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 01:05:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 01:05:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 01:07:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 01:08:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 01:09:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 01:11:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 01:13:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Nov 21 01:13:49 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -718,7 +979,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>142</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>23</v>
@@ -823,7 +1084,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>152</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -920,7 +1181,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>160</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1017,7 +1278,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>150</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1114,7 +1375,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1211,7 +1472,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1308,7 +1569,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1405,7 +1666,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1502,7 +1763,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1599,7 +1860,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1696,7 +1957,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1793,7 +2054,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>23</v>
@@ -1892,7 +2153,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -1989,7 +2250,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2083,10 +2344,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2183,7 +2444,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2280,7 +2541,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2377,7 +2638,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2474,7 +2735,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>124</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2571,7 +2832,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>125</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2668,7 +2929,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2765,7 +3026,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>131</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2862,7 +3123,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2959,7 +3220,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>135</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -3056,7 +3317,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>138</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -3152,6 +3413,12 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>159</v>
+      </c>
       <c r="C2" s="3" t="s">
         <v>27</v>
       </c>
@@ -3249,10 +3516,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -3352,7 +3619,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -3449,7 +3716,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -3549,7 +3816,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -3646,7 +3913,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>163</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -3743,7 +4010,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>170</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -3840,7 +4107,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>162</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -3937,7 +4204,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -4034,7 +4301,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>165</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -4127,6 +4394,12 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>169</v>
+      </c>
       <c r="C2" s="3" t="s">
         <v>29</v>
       </c>
@@ -4224,7 +4497,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>118</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -4321,7 +4594,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -4418,7 +4691,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -4515,7 +4788,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>148</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -4615,7 +4888,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -4712,7 +4985,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -4809,10 +5082,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>113</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -4912,7 +5185,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>147</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Added Test Cases in BWP
</commit_message>
<xml_diff>
--- a/KatalonData/BWPBootstrapData/BWPACHData.xlsx
+++ b/KatalonData/BWPBootstrapData/BWPACHData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476046\Documents\VPS-Katalon-feature-VRelay\KatalonData\BWPBootstrapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925EEBDC-DC61-49C0-B90D-65CD0CBFF969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E1A0A7-BC18-4D8D-8BEC-EB12C7564819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="24" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="27" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PayNowCorpNoCF" sheetId="1" r:id="rId1"/>
@@ -40,25 +40,29 @@
     <sheet name="SingleCFCeilingPC" sheetId="37" r:id="rId25"/>
     <sheet name="MissingReqFieldsCorp" sheetId="45" r:id="rId26"/>
     <sheet name="MissingReqFieldsPersonalACH" sheetId="46" r:id="rId27"/>
-    <sheet name="SingleCFFlatCorp" sheetId="39" r:id="rId28"/>
-    <sheet name="SingleCFFlatPC" sheetId="40" r:id="rId29"/>
-    <sheet name="SingleCFFlatPS" sheetId="41" r:id="rId30"/>
-    <sheet name="SingleCFPercentageCorp" sheetId="42" r:id="rId31"/>
-    <sheet name="SingleCFPercentagePC" sheetId="43" r:id="rId32"/>
-    <sheet name="SingleCFPercentagePS" sheetId="44" r:id="rId33"/>
-    <sheet name="PayNowPCNoCFReqFields" sheetId="4" r:id="rId34"/>
-    <sheet name="PayNowPCNoCFOnly" sheetId="14" r:id="rId35"/>
-    <sheet name="NoModifyAmountPC" sheetId="17" r:id="rId36"/>
-    <sheet name="MinAmountErrorPC" sheetId="23" r:id="rId37"/>
-    <sheet name="MaxAmountErrorPC" sheetId="20" r:id="rId38"/>
-    <sheet name="PayNowPSNoCF" sheetId="5" r:id="rId39"/>
-    <sheet name="PayNowPSSCF" sheetId="10" r:id="rId40"/>
-    <sheet name="PayNowPSDCF" sheetId="12" r:id="rId41"/>
-    <sheet name="PayNowPSNoCFOnly" sheetId="15" r:id="rId42"/>
-    <sheet name="PayNowPSNoCFReqFields" sheetId="6" r:id="rId43"/>
-    <sheet name="NoModifyAmountPS" sheetId="18" r:id="rId44"/>
-    <sheet name="MaxAmountErrorPS" sheetId="21" r:id="rId45"/>
-    <sheet name="MinAmountErrorPS" sheetId="24" r:id="rId46"/>
+    <sheet name="ModifyPaymentsCorp1" sheetId="47" r:id="rId28"/>
+    <sheet name="ModifyPaymentsCorp2" sheetId="48" r:id="rId29"/>
+    <sheet name="ModifyPaymentsPC1" sheetId="49" r:id="rId30"/>
+    <sheet name="ModifyPaymentsPC2" sheetId="50" r:id="rId31"/>
+    <sheet name="SingleCFFlatCorp" sheetId="39" r:id="rId32"/>
+    <sheet name="SingleCFFlatPC" sheetId="40" r:id="rId33"/>
+    <sheet name="SingleCFFlatPS" sheetId="41" r:id="rId34"/>
+    <sheet name="SingleCFPercentageCorp" sheetId="42" r:id="rId35"/>
+    <sheet name="SingleCFPercentagePC" sheetId="43" r:id="rId36"/>
+    <sheet name="SingleCFPercentagePS" sheetId="44" r:id="rId37"/>
+    <sheet name="PayNowPCNoCFReqFields" sheetId="4" r:id="rId38"/>
+    <sheet name="PayNowPCNoCFOnly" sheetId="14" r:id="rId39"/>
+    <sheet name="NoModifyAmountPC" sheetId="17" r:id="rId40"/>
+    <sheet name="MinAmountErrorPC" sheetId="23" r:id="rId41"/>
+    <sheet name="MaxAmountErrorPC" sheetId="20" r:id="rId42"/>
+    <sheet name="PayNowPSNoCF" sheetId="5" r:id="rId43"/>
+    <sheet name="PayNowPSSCF" sheetId="10" r:id="rId44"/>
+    <sheet name="PayNowPSDCF" sheetId="12" r:id="rId45"/>
+    <sheet name="PayNowPSNoCFOnly" sheetId="15" r:id="rId46"/>
+    <sheet name="PayNowPSNoCFReqFields" sheetId="6" r:id="rId47"/>
+    <sheet name="NoModifyAmountPS" sheetId="18" r:id="rId48"/>
+    <sheet name="MaxAmountErrorPS" sheetId="21" r:id="rId49"/>
+    <sheet name="MinAmountErrorPS" sheetId="24" r:id="rId50"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -70,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="88">
   <si>
     <t>Result</t>
   </si>
@@ -331,6 +335,9 @@
   </si>
   <si>
     <t>17</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
@@ -671,7 +678,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="A1:XFD1048576"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,7 +783,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="A1:XFD1048576"/>
+      <selection activeCell="F9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2523,7 +2530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E5825C-6EEF-49AA-9880-B92945E2442C}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
@@ -2614,14 +2621,17 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB610E4-D8A9-4F86-99AA-691BCAA68B9C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B10A84-4465-4F3C-AB05-F2529380B3EA}">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="26" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -2668,21 +2678,17 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>16</v>
@@ -2711,14 +2717,17 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3C025A-C3F4-4ABF-9C60-AA1DCCB0BC50}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD262109-C636-4152-9E03-BF0F49D8C917}">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="26" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -2769,17 +2778,19 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>16</v>
@@ -2789,10 +2800,10 @@
         <v>17</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
@@ -2905,6 +2916,400 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FBEB25C-002A-46ED-B528-BBFB127AD6B5}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A3C05C-8E29-42C3-A89E-8ED671B7BB31}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB610E4-D8A9-4F86-99AA-691BCAA68B9C}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3C025A-C3F4-4ABF-9C60-AA1DCCB0BC50}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A067396-2824-448F-9289-4B8D3E2041FE}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -3001,7 +3406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AECE1F9-32F0-48E5-B835-168A7EF42FA8}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -3098,7 +3503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEB8BAF-D441-4510-B01C-E6A2F0E35EEA}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -3195,7 +3600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4CCB5A6-D07A-4BC3-BD3B-767113A862D2}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -3292,7 +3697,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F93338-8AAA-4B19-8B9D-4771302FEFC0}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -3394,7 +3799,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EC6E653-D4E4-4FCF-8BD0-11D4CBABA3A9}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -3480,400 +3885,6 @@
       </c>
       <c r="K2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF98BAE0-3DBA-4724-A623-84E06EAD3F5D}">
-  <dimension ref="A1:N2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CD5E31-F635-4FC0-9668-1419F01D6942}">
-  <dimension ref="A1:N2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD2F0AE-7828-442C-A2B3-21D0EBE7331D}">
-  <dimension ref="A1:N2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E2C147-58C7-49F8-940A-3E37DE049451}">
-  <dimension ref="A1:N2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
@@ -3986,6 +3997,400 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF98BAE0-3DBA-4724-A623-84E06EAD3F5D}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CD5E31-F635-4FC0-9668-1419F01D6942}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD2F0AE-7828-442C-A2B3-21D0EBE7331D}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E2C147-58C7-49F8-940A-3E37DE049451}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC79200-E4B3-4160-86F6-78B06F6EA2C0}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -4082,7 +4487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{026E9C75-7C58-441D-91D6-25552A135B0A}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -4179,7 +4584,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D307F9B9-84A6-4F70-AF5F-E09C0B70177D}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -4276,7 +4681,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CED210A-15BA-4154-A75C-369A0BF113DA}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -4375,7 +4780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CCEC20-911A-47BC-B790-0438DD3BE26D}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -4472,7 +4877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE927C8-204D-43C3-9530-F9F77785B40B}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -4539,103 +4944,6 @@
       </c>
       <c r="E2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAABB2E9-54E4-4860-85B4-28F35D889E47}">
-  <dimension ref="A1:N2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>15</v>
@@ -4755,6 +5063,103 @@
         <v>18</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAABB2E9-54E4-4860-85B4-28F35D889E47}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>